<commit_message>
Add DAC signal calculations
</commit_message>
<xml_diff>
--- a/documents/calculations.xlsx
+++ b/documents/calculations.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
     <sheet name="Low pass filters" sheetId="2" r:id="rId2"/>
+    <sheet name="Wave approximations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Fosc</t>
   </si>
@@ -85,6 +86,18 @@
   </si>
   <si>
     <t>Cutoff frequency</t>
+  </si>
+  <si>
+    <t>2 pii</t>
+  </si>
+  <si>
+    <t>0 to 1</t>
+  </si>
+  <si>
+    <t>2 pii * 0to1</t>
+  </si>
+  <si>
+    <t>SINE WAVE</t>
   </si>
 </sst>
 </file>
@@ -758,7 +771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -800,7 +813,7 @@
         <v>2.2000000000000001E-7</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C15" si="0">1/(2*3.141592*A3*B3)</f>
+        <f t="shared" ref="C3:C4" si="0">1/(2*3.141592*A3*B3)</f>
         <v>72.343171001430875</v>
       </c>
     </row>
@@ -819,4 +832,367 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:V7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4">
+        <f>2*PI()</f>
+        <v>6.2831853071795862</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0.05</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E4">
+        <v>0.15</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G4">
+        <v>0.25</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="I4">
+        <v>0.35</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="K4">
+        <v>0.45</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="M4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O4">
+        <v>0.65</v>
+      </c>
+      <c r="P4" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="Q4">
+        <v>0.75</v>
+      </c>
+      <c r="R4" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="S4">
+        <v>0.85</v>
+      </c>
+      <c r="T4" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="U4">
+        <v>0.95</v>
+      </c>
+      <c r="V4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <f>$B$1*B4</f>
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:L5" si="0">$B$1*C4</f>
+        <v>0.31415926535897931</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.62831853071795862</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.94247779607693793</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1.2566370614359172</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>1.8849555921538759</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>2.1991148575128552</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>2.5132741228718345</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>2.8274333882308138</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5" si="1">$B$1*M4</f>
+        <v>3.4557519189487729</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5" si="2">$B$1*N4</f>
+        <v>3.7699111843077517</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5" si="3">$B$1*O4</f>
+        <v>4.0840704496667311</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5" si="4">$B$1*P4</f>
+        <v>4.3982297150257104</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ref="Q5" si="5">$B$1*Q4</f>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5" si="6">$B$1*R4</f>
+        <v>5.026548245743669</v>
+      </c>
+      <c r="S5">
+        <f t="shared" ref="S5" si="7">$B$1*S4</f>
+        <v>5.3407075111026483</v>
+      </c>
+      <c r="T5">
+        <f t="shared" ref="T5" si="8">$B$1*T4</f>
+        <v>5.6548667764616276</v>
+      </c>
+      <c r="U5">
+        <f t="shared" ref="U5" si="9">$B$1*U4</f>
+        <v>5.9690260418206069</v>
+      </c>
+      <c r="V5">
+        <f t="shared" ref="V5" si="10">$B$1*V4</f>
+        <v>6.2831853071795862</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <f>ROUND(128 + 127*SIN(B5),0)</f>
+        <v>128</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:V7" si="11">ROUND(128 + 127*SIN(C5),0)</f>
+        <v>167</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="11"/>
+        <v>203</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="11"/>
+        <v>231</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="11"/>
+        <v>249</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="11"/>
+        <v>255</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="11"/>
+        <v>249</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="11"/>
+        <v>231</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="11"/>
+        <v>203</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="11"/>
+        <v>167</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="11"/>
+        <v>128</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="11"/>
+        <v>89</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="11"/>
+        <v>53</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="11"/>
+        <v>53</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="11"/>
+        <v>89</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="11"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <f>128 + 127*SIN(B6)</f>
+        <v>128</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C7:V8" si="12">128 + 127*SIN(C6)</f>
+        <v>128</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update calculations and add a program plan
</commit_message>
<xml_diff>
--- a/documents/calculations.xlsx
+++ b/documents/calculations.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
     <sheet name="Low pass filters" sheetId="2" r:id="rId2"/>
     <sheet name="Wave approximations" sheetId="3" r:id="rId3"/>
+    <sheet name="Moottorin pyörimisnopeus laskut" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Fosc</t>
   </si>
@@ -98,6 +99,24 @@
   </si>
   <si>
     <t>SINE WAVE</t>
+  </si>
+  <si>
+    <t>Kierron delay</t>
+  </si>
+  <si>
+    <t>motorDelay</t>
+  </si>
+  <si>
+    <t>motorStepDelay</t>
+  </si>
+  <si>
+    <t>Askelia per kierros</t>
+  </si>
+  <si>
+    <t>kierroksen pituus</t>
+  </si>
+  <si>
+    <t>kiertonopeus</t>
   </si>
 </sst>
 </file>
@@ -838,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:V7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,7 +1130,7 @@
         <v>128</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C7:V8" si="12">128 + 127*SIN(C6)</f>
+        <f t="shared" ref="C8:V8" si="12">128 + 127*SIN(C6)</f>
         <v>128</v>
       </c>
       <c r="D8">
@@ -1195,4 +1214,230 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="B2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>128</v>
+      </c>
+      <c r="D4">
+        <v>256</v>
+      </c>
+      <c r="E4">
+        <v>512</v>
+      </c>
+      <c r="F4">
+        <v>1024</v>
+      </c>
+      <c r="G4">
+        <f>2*F4</f>
+        <v>2048</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:M4" si="0">2*G4</f>
+        <v>4096</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>8192</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>16384</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>32768</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <f>$A$2*B4</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:I5" si="1">$A$2*C4</f>
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>5.1200000000000002E-2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>0.1024</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.20480000000000001</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0.40960000000000002</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>0.81920000000000004</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>1.6384000000000001</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5" si="2">$A$2*J4</f>
+        <v>3.2768000000000002</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5" si="3">$A$2*K4</f>
+        <v>6.5536000000000003</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5" si="4">$A$2*L4</f>
+        <v>13.107200000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <f>$B$2*B5</f>
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:L6" si="5">$B$2*C5</f>
+        <v>0.81920000000000004</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="5"/>
+        <v>1.6384000000000001</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="5"/>
+        <v>3.2768000000000002</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="5"/>
+        <v>6.5536000000000003</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="5"/>
+        <v>13.107200000000001</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="5"/>
+        <v>26.214400000000001</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="5"/>
+        <v>52.428800000000003</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="5"/>
+        <v>104.85760000000001</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="5"/>
+        <v>209.71520000000001</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="5"/>
+        <v>419.43040000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <f>1/B6</f>
+        <v>156.25</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:L7" si="6">1/C6</f>
+        <v>1.220703125</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="6"/>
+        <v>0.6103515625</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="6"/>
+        <v>0.30517578125</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="6"/>
+        <v>0.152587890625</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="6"/>
+        <v>7.62939453125E-2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="6"/>
+        <v>3.814697265625E-2</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="6"/>
+        <v>1.9073486328125E-2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="6"/>
+        <v>9.5367431640625E-3</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="6"/>
+        <v>4.76837158203125E-3</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="6"/>
+        <v>2.384185791015625E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>